<commit_message>
自动更新Excel文件 - Sat Jul  5 03:52:49 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -475,7 +475,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="n">
         <v>20250705</v>
@@ -496,7 +496,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="n">
         <v>20250705</v>
@@ -517,7 +517,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" t="n">
         <v>20250704</v>
@@ -538,7 +538,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="n">
         <v>20250704</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Sep 29 23:22:11 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,10 +498,10 @@
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
-        <v>20250928</v>
+        <v>20250926</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>10</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
-        <v>20250928</v>
+        <v>20250926</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>10</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
-        <v>20250928</v>
+        <v>20250926</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
-        <v>20250928</v>
+        <v>20250926</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -635,19 +635,15 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
-        <v>20250923</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>大桶1个</t>
-        </is>
-      </c>
+        <v>20250926</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>小桶1个</t>
@@ -673,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
-        <v>20250928</v>
+        <v>20250926</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -704,10 +700,10 @@
         <v>10</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
-        <v>20250928</v>
+        <v>20250926</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -735,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
-        <v>20250928</v>
+        <v>20250926</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -766,16 +762,12 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
-        <v>20250923</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>大桶1个</t>
-        </is>
-      </c>
+        <v>20250926</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
           <t>小桶1个</t>
@@ -801,10 +793,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
-        <v>20250928</v>
+        <v>20250926</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -829,19 +821,15 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
-        <v>20250923</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>大桶1个</t>
-        </is>
-      </c>
+        <v>20250926</v>
+      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
           <t>小桶1个</t>
@@ -867,10 +855,10 @@
         <v>10</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
-        <v>20250928</v>
+        <v>20250926</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -902,10 +890,10 @@
         <v>10</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
-        <v>20250928</v>
+        <v>20250926</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -937,10 +925,10 @@
         <v>10</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
-        <v>20250928</v>
+        <v>20250926</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -972,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20250928</v>
@@ -1003,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
-        <v>20250928</v>
+        <v>20250925</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1034,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1065,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1096,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1127,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1158,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1189,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
-        <v>20250928</v>
+        <v>20250925</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1220,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
-        <v>20250928</v>
+        <v>20250925</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1251,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
-        <v>20250928</v>
+        <v>20250921</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1282,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
-        <v>20250928</v>
+        <v>20250925</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1313,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20250923</v>
@@ -1348,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1379,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1410,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1441,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1472,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1503,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1534,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1569,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20250919</v>
+        <v>20250929</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1600,7 +1588,7 @@
         <v>10</v>
       </c>
       <c r="E36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F36" t="n">
         <v>20250921</v>
@@ -1631,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20250921</v>
@@ -1662,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20250921</v>
@@ -1693,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20250921</v>
@@ -1731,7 +1719,7 @@
         <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20250928</v>
+        <v>20250929</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1762,7 +1750,7 @@
         <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20250928</v>
+        <v>20250929</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1790,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20250921</v>
@@ -1818,13 +1806,13 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
-        <v>20250928</v>
+        <v>20250921</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1855,7 +1843,7 @@
         <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20250928</v>
+        <v>20250929</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1883,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
-        <v>20250923</v>
+        <v>20250925</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1911,13 +1899,13 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20250923</v>
+        <v>20250929</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1949,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20250923</v>
@@ -1983,7 +1971,7 @@
         <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20250928</v>
+        <v>20250929</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -2011,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20250922</v>
+        <v>20250929</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2042,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
-        <v>20250928</v>
+        <v>20250924</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2073,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
-        <v>20250928</v>
+        <v>20250924</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2104,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
-        <v>20250928</v>
+        <v>20250924</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2135,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
-        <v>20250928</v>
+        <v>20250924</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2166,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
-        <v>20250928</v>
+        <v>20250924</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2197,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
-        <v>20250928</v>
+        <v>20250924</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2225,13 +2213,13 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
-        <v>20250923</v>
+        <v>20250924</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2259,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
-        <v>20250928</v>
+        <v>20250924</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2287,13 +2275,13 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
-        <v>20250924</v>
+        <v>20250928</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2321,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20250928</v>
@@ -2352,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20250928</v>
@@ -2383,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20250924</v>
+        <v>20250929</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2414,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20250928</v>
@@ -2445,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20250928</v>
@@ -2476,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20250928</v>
@@ -2507,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20250928</v>
@@ -2535,13 +2523,13 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20250928</v>
+        <v>20250929</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2566,13 +2554,13 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20250928</v>
+        <v>20250929</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2603,7 +2591,7 @@
         <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20250928</v>
+        <v>20250929</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2634,7 +2622,7 @@
         <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20250928</v>
+        <v>20250929</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2662,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20250920</v>
@@ -2693,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20250920</v>
@@ -2724,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20250920</v>
@@ -2755,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20250920</v>
@@ -2786,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20250920</v>
@@ -2817,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20250920</v>
@@ -2848,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20250920</v>
@@ -2879,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20250921</v>
@@ -2910,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20250921</v>
@@ -2941,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20250921</v>
@@ -2953,6 +2941,436 @@
       </c>
       <c r="H79" t="inlineStr"/>
       <c r="I79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>周广平特色</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>大湖大街</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>10</v>
+      </c>
+      <c r="E80" t="n">
+        <v>4</v>
+      </c>
+      <c r="F80" t="n">
+        <v>20250923</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>大桶1个</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>食惠坊</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>大湖大街</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>10</v>
+      </c>
+      <c r="E81" t="n">
+        <v>4</v>
+      </c>
+      <c r="F81" t="n">
+        <v>20250923</v>
+      </c>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>小桶1个</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>味满堂</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>大湖大街</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>10</v>
+      </c>
+      <c r="E82" t="n">
+        <v>4</v>
+      </c>
+      <c r="F82" t="n">
+        <v>20250923</v>
+      </c>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>小桶1个</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>社区家常菜</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>大湖大街</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>10</v>
+      </c>
+      <c r="E83" t="n">
+        <v>4</v>
+      </c>
+      <c r="F83" t="n">
+        <v>20250923</v>
+      </c>
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>小桶1个</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>淮扬面馆</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>崇义路</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>10</v>
+      </c>
+      <c r="E84" t="n">
+        <v>4</v>
+      </c>
+      <c r="F84" t="n">
+        <v>20250923</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>大桶1个</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>金陵水饺城</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>平阳东路</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>10</v>
+      </c>
+      <c r="E85" t="n">
+        <v>4</v>
+      </c>
+      <c r="F85" t="n">
+        <v>20250923</v>
+      </c>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>小桶1个</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>大路全羊</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>崇义路</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>10</v>
+      </c>
+      <c r="E86" t="n">
+        <v>4</v>
+      </c>
+      <c r="F86" t="n">
+        <v>20250923</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>大桶1个</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>范大碗</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>平阳路</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>7</v>
+      </c>
+      <c r="E87" t="n">
+        <v>2</v>
+      </c>
+      <c r="F87" t="n">
+        <v>20250924</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>大桶4个</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>微渔坊</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>峄山路</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>7</v>
+      </c>
+      <c r="E88" t="n">
+        <v>5</v>
+      </c>
+      <c r="F88" t="n">
+        <v>20250927</v>
+      </c>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>小桶2个</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>澳龙特色餐厅</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>崇义路</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>7</v>
+      </c>
+      <c r="E89" t="n">
+        <v>5</v>
+      </c>
+      <c r="F89" t="n">
+        <v>20250927</v>
+      </c>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>小桶4个</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>福源酒家</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>峄山路</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>7</v>
+      </c>
+      <c r="E90" t="n">
+        <v>6</v>
+      </c>
+      <c r="F90" t="n">
+        <v>20250928</v>
+      </c>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>小桶2个</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>九道菜</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>峄山路</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>7</v>
+      </c>
+      <c r="E91" t="n">
+        <v>6</v>
+      </c>
+      <c r="F91" t="n">
+        <v>20250928</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>大桶1个</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr"/>
+      <c r="I91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>百大生态园</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>峄山路</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>7</v>
+      </c>
+      <c r="E92" t="n">
+        <v>6</v>
+      </c>
+      <c r="F92" t="n">
+        <v>20250928</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>大桶5个</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr"/>
+      <c r="I92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>顺合庭私厨大湖大街</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="n">
+        <v>10</v>
+      </c>
+      <c r="E93" t="n">
+        <v>4</v>
+      </c>
+      <c r="F93" t="n">
+        <v>20250923</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>大桶2个</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Oct  7 23:21:54 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251006</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20250930</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20250929</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20250929</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20250929</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20250929</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251007</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20250929</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20250929</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20250929</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20250929</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20250929</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20250929</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20250929</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20250929</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20250929</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20250929</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20250929</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251006</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251006</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20250929</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251006</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251006</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20250929</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251006</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251007</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251004</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251004</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251004</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251004</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251004</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251004</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251004</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251004</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20250928</v>
+        <v>20251008</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20250928</v>
+        <v>20251008</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20250928</v>
+        <v>20251008</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251007</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20250928</v>
+        <v>20251008</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20250928</v>
+        <v>20251008</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20250928</v>
+        <v>20251008</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20250929</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20250929</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20250929</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20250929</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20250929</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20250930</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20250930</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20250930</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20250930</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20250930</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20250930</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20250930</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251003</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251003</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251003</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251003</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251003</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251003</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251003</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251003</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251003</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251003</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251006</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251006</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251006</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251006</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251006</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251003</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251002</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251002</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Oct  8 23:21:59 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251006</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20250930</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251007</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251006</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251006</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251006</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251006</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251006</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251007</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251004</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251004</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251004</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251004</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251004</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251004</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251004</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251004</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251007</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20250929</v>
+        <v>20251009</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20250930</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20250930</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20250930</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20250930</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20250930</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20250930</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20250930</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251003</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251003</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251003</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251003</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251003</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251003</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251003</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251003</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251003</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251003</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251006</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251006</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251006</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251006</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251006</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251003</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251002</v>
+        <v>20251009</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251002</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Oct  9 23:21:41 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251006</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251007</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251006</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251006</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251006</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251006</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251006</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251007</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251004</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251004</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251004</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251004</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251004</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251004</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251004</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251004</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251007</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20250930</v>
+        <v>20251010</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251003</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251003</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251003</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251003</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251003</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251003</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251003</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251003</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251003</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251003</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251006</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251006</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251006</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251006</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251006</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251003</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251009</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251002</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Oct 10 23:21:13 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251006</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251007</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251006</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251006</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251006</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251006</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251006</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251007</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251004</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251004</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251004</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251004</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251004</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251004</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251004</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251004</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251007</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251003</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251003</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251003</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251003</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251003</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251003</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251003</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251003</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251003</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251003</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251006</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251006</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251006</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251006</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251006</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251003</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251009</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251002</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Oct 11 23:21:45 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251006</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251007</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251006</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251006</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251006</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251006</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251006</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251007</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251004</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251004</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251004</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251004</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251004</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251004</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251004</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251004</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251007</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251003</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251003</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251003</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251003</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251003</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251003</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251003</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251003</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251003</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251003</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251006</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251006</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251006</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251006</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251006</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251003</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251009</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251002</v>
+        <v>20251012</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Oct 12 23:21:27 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251006</v>
+        <v>20251013</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251007</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251006</v>
+        <v>20251013</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251006</v>
+        <v>20251013</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251006</v>
+        <v>20251013</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251006</v>
+        <v>20251013</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251006</v>
+        <v>20251013</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251007</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251004</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251004</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251004</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251004</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251004</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251004</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251004</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251004</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251007</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251003</v>
+        <v>20251013</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251003</v>
+        <v>20251013</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251003</v>
+        <v>20251013</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251003</v>
+        <v>20251013</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251003</v>
+        <v>20251013</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251003</v>
+        <v>20251013</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251003</v>
+        <v>20251013</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251003</v>
+        <v>20251013</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251003</v>
+        <v>20251013</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251003</v>
+        <v>20251013</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251006</v>
+        <v>20251013</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251006</v>
+        <v>20251013</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251006</v>
+        <v>20251013</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251006</v>
+        <v>20251013</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251006</v>
+        <v>20251013</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251003</v>
+        <v>20251013</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251009</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3437,6 +3437,130 @@
       </c>
       <c r="H95" t="inlineStr"/>
       <c r="I95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>俏大姐</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>唐王河路（小湖美食城）</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>10</v>
+      </c>
+      <c r="E96" t="n">
+        <v>7</v>
+      </c>
+      <c r="F96" t="n">
+        <v>20251010</v>
+      </c>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>小桶1个</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>西子居</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>体育馆</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>10</v>
+      </c>
+      <c r="E97" t="n">
+        <v>7</v>
+      </c>
+      <c r="F97" t="n">
+        <v>20251010</v>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>大桶2个</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr"/>
+      <c r="I97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>德胜园</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>邾国大道</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>10</v>
+      </c>
+      <c r="E98" t="n">
+        <v>7</v>
+      </c>
+      <c r="F98" t="n">
+        <v>20251010</v>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>大桶1个</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr"/>
+      <c r="I98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>老鲁味</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>唐王河路（小湖美食城）</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>10</v>
+      </c>
+      <c r="E99" t="n">
+        <v>7</v>
+      </c>
+      <c r="F99" t="n">
+        <v>20251010</v>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>大桶1个</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Oct 13 23:21:34 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251013</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251007</v>
+        <v>20251014</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251013</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251013</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251013</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251013</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251013</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251007</v>
+        <v>20251014</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251004</v>
+        <v>20251014</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251007</v>
+        <v>20251014</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251013</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251013</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251013</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251013</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251013</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251009</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251010</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251010</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251010</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251010</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Oct 14 23:22:33 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251006</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251006</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251006</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251013</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251006</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251006</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251006</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251006</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251006</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251006</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251006</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251014</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251013</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251013</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251006</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251013</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251006</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251013</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251013</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251014</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251014</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251013</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251013</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251013</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251013</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251006</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251013</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251009</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251010</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251010</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251010</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251010</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Oct 15 23:21:52 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251013</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251014</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251013</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251013</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251013</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251013</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251013</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251014</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251014</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251013</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251013</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251013</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251013</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251006</v>
+        <v>20251016</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251013</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251009</v>
+        <v>20251016</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251010</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251010</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251010</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251010</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Oct 16 23:19:57 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251013</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251014</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251013</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251013</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251013</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251013</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251013</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251014</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251008</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251008</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251008</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251014</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251008</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251008</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251008</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251013</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251013</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251013</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251013</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251013</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251016</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251010</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251010</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251010</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251010</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Oct 17 23:21:50 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251013</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251009</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251009</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251009</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251009</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251014</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251009</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251009</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251009</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251009</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251009</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251009</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251009</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251009</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251009</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251009</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251009</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251013</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251013</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251009</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251013</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251013</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251009</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251013</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251014</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251008</v>
+        <v>20251018</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251008</v>
+        <v>20251018</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251008</v>
+        <v>20251018</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251014</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251008</v>
+        <v>20251018</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251008</v>
+        <v>20251018</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251008</v>
+        <v>20251018</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251009</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251009</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251009</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251009</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251009</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251013</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251013</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251013</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251013</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251013</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251016</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251010</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251010</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251010</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251010</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Oct 18 23:21:57 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251006</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251006</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251006</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251006</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251006</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251013</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251006</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251006</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251006</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251006</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251010</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251014</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251013</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251013</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251013</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251013</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251013</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251014</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251014</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251009</v>
+        <v>20251019</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251010</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251010</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251010</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251010</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251010</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251010</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251010</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251013</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251013</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251013</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251013</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251013</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251016</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251010</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251010</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251010</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251010</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Oct 19 23:22:14 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251006</v>
+        <v>20251020</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251014</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251014</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251014</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251013</v>
+        <v>20251020</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251016</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251010</v>
+        <v>20251020</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Oct 20 23:22:22 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251020</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251014</v>
+        <v>20251021</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251020</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251020</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251020</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251020</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251020</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251014</v>
+        <v>20251021</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251014</v>
+        <v>20251021</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251020</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251020</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251020</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251020</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251020</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251016</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251012</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Oct 21 23:23:54 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251020</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251021</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251020</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251020</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251020</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251020</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251020</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251021</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251021</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251013</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251013</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251013</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251013</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251013</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251013</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251013</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251013</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251013</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251013</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251020</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251020</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251020</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251020</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251020</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251013</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251016</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251012</v>
+        <v>20251022</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Oct 22 23:21:41 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251020</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251021</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251020</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251020</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251020</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251020</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251020</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251021</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251014</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251014</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251014</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251014</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251014</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251014</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251014</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251014</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251021</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251020</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251020</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251020</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251020</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251020</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251013</v>
+        <v>20251023</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251016</v>
+        <v>20251023</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Oct 23 23:22:09 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251020</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251021</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251020</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251020</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251020</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251020</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251020</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251021</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251014</v>
+        <v>20251024</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251021</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251020</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251020</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251020</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251020</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251020</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251023</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Oct 24 23:23:04 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251016</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251016</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251016</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251020</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251016</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251016</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251016</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251016</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251016</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251016</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251016</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251021</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251020</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251020</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251016</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251020</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251016</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251020</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251020</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251021</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251021</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251020</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251020</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251020</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251020</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251016</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251020</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251023</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Oct 25 23:21:29 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251020</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251021</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251020</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251020</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251020</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251020</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251020</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251021</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251021</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251020</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251020</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251020</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251020</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251016</v>
+        <v>20251026</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251020</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251023</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Oct 26 23:22:51 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251021</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251021</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251018</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251018</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251018</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251021</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251018</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251018</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251018</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251020</v>
+        <v>20251027</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251023</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Oct 27 23:22:54 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251027</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251019</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251019</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251019</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251019</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251021</v>
+        <v>20251028</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251019</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251019</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251019</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251019</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251019</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251019</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251019</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251019</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251019</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251019</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251019</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251027</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251027</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251019</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251027</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251027</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251019</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251027</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251021</v>
+        <v>20251028</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251018</v>
+        <v>20251028</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251018</v>
+        <v>20251028</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251018</v>
+        <v>20251028</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251021</v>
+        <v>20251028</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251018</v>
+        <v>20251028</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251018</v>
+        <v>20251028</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251018</v>
+        <v>20251028</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251019</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251019</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251019</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251019</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251019</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251027</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251027</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251027</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251027</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251027</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251023</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Oct 28 23:23:48 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251027</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251020</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251028</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251027</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251027</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251027</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251027</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251027</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251028</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251028</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251019</v>
+        <v>20251029</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251020</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251020</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251020</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251020</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251020</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251020</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251020</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251027</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251027</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251027</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251027</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251027</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251023</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251020</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251020</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251020</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251020</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Oct 29 23:24:04 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251027</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251028</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251027</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251027</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251027</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251027</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251027</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251028</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251028</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251027</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251027</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251027</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251027</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251027</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251023</v>
+        <v>20251030</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251020</v>
+        <v>20251030</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Oct 30 23:23:06 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251027</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251028</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251027</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251027</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251027</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251027</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251027</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251028</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251028</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251027</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251027</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251027</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251027</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251027</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251030</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251022</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Oct 31 23:23:07 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251027</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251028</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251027</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251027</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251027</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251027</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251027</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251028</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251028</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251023</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251023</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251023</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251023</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251023</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251023</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251023</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251023</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251023</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251023</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251027</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251027</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251027</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251027</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251027</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251023</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251030</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251022</v>
+        <v>20251101</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Nov  1 23:22:06 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251020</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251020</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251020</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251020</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251020</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251027</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251020</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251020</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251020</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251020</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251028</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251027</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251027</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251027</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251027</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251027</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251028</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251024</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251024</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251024</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251024</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251024</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251024</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251024</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251024</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251028</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251027</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251027</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251027</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251027</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251027</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251023</v>
+        <v>20251102</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251030</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Nov  2 23:22:20 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251020</v>
+        <v>20251103</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251028</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251028</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251024</v>
+        <v>20251103</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251028</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251027</v>
+        <v>20251103</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251030</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Nov  3 23:23:55 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251026</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251026</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251026</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251103</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251026</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251026</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251026</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251026</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251026</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251026</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251026</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251028</v>
+        <v>20251104</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251103</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251103</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251026</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251103</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251026</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251103</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251103</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251028</v>
+        <v>20251104</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251028</v>
+        <v>20251104</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251103</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251103</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251103</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251103</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251026</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251103</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251030</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Nov  4 23:23:52 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251103</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251104</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251103</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251103</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251103</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251103</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251103</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251104</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251104</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251103</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251103</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251103</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251103</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251026</v>
+        <v>20251105</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251103</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251030</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Nov  5 23:24:07 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251103</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251104</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251103</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251103</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251103</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251103</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251103</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251104</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251028</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251028</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251028</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251104</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251028</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251028</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251028</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251103</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251103</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251103</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251103</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251103</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251030</v>
+        <v>20251106</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Nov  6 23:23:34 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251103</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251029</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251029</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251029</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251029</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251104</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251029</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251029</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251029</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251029</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251029</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251029</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251029</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251029</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251029</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251029</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251029</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251103</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251103</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251029</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251103</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251103</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251029</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251103</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251104</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251028</v>
+        <v>20251107</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251028</v>
+        <v>20251107</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251028</v>
+        <v>20251107</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251104</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251028</v>
+        <v>20251107</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251028</v>
+        <v>20251107</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251028</v>
+        <v>20251107</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251029</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251029</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251029</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251029</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251029</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251103</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251103</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251103</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251103</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251103</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251106</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Nov  7 23:23:05 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251103</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251030</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251104</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251103</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251103</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251103</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251103</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251103</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251104</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251104</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251029</v>
+        <v>20251108</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251030</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251030</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251030</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251030</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251030</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251030</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251030</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251103</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251103</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251103</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251103</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251103</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251106</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251030</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251030</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251030</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251030</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Nov  8 23:22:09 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251103</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251104</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251103</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251103</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251103</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251103</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251103</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251104</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251104</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251103</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251103</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251103</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251103</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251103</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251106</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251030</v>
+        <v>20251109</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Nov  9 23:22:27 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251104</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251104</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251104</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251103</v>
+        <v>20251110</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251106</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251101</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Nov 10 23:24:34 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251110</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251104</v>
+        <v>20251111</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251110</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251110</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251110</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251110</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251110</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251104</v>
+        <v>20251111</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251104</v>
+        <v>20251111</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251102</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251102</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251102</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251102</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251102</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251102</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251102</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251102</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251102</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251102</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251110</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251110</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251110</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251110</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251110</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251102</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251106</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251101</v>
+        <v>20251111</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Nov 11 23:23:42 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251110</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251111</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251110</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251110</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251110</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251110</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251110</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251111</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251103</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251103</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251103</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251103</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251103</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251103</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251103</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251103</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251111</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251110</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251110</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251110</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251110</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251110</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251102</v>
+        <v>20251112</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251106</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Nov 12 23:25:01 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251110</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251111</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251110</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251110</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251110</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251110</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251110</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251111</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251103</v>
+        <v>20251113</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251111</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251110</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251110</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251110</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251110</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251110</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251106</v>
+        <v>20251113</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Nov 13 23:25:08 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251105</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251105</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251105</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251110</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251105</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251105</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251105</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251105</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251105</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251105</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251105</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251111</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251110</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251110</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251105</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251110</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251105</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251110</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251110</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251111</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251111</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251110</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251110</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251110</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251110</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251105</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251110</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251113</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Nov 14 23:23:26 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251110</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251111</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251110</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251110</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251110</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251110</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251110</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251111</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251111</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251110</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251110</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251110</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251110</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251105</v>
+        <v>20251115</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251110</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251113</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Nov 15 23:23:16 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251103</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251103</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251103</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251103</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251103</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251110</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251103</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251103</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251103</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251103</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251111</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251110</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251110</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251110</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251110</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251110</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251111</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251107</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251107</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251107</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251111</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251107</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251107</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251107</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251110</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251110</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251110</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251110</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251110</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251113</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Nov 16 23:23:17 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251103</v>
+        <v>20251117</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251108</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251108</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251108</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251108</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251111</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251108</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251108</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251108</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251108</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251108</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251108</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251108</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251108</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251108</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251108</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251108</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251108</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251108</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251111</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251107</v>
+        <v>20251117</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251107</v>
+        <v>20251117</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251107</v>
+        <v>20251117</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251111</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251107</v>
+        <v>20251117</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251107</v>
+        <v>20251117</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251107</v>
+        <v>20251117</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251108</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251108</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251108</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251108</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251108</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251110</v>
+        <v>20251117</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251113</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Nov 17 23:24:26 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251117</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251109</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251111</v>
+        <v>20251118</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251117</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251117</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251117</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251117</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251117</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251111</v>
+        <v>20251118</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251111</v>
+        <v>20251118</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251108</v>
+        <v>20251118</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251109</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251109</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251109</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251109</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251109</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251109</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251109</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251117</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251117</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251117</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251117</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251117</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251113</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251109</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251109</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251109</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251109</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Nov 18 23:24:07 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251117</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251118</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251117</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251117</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251117</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251117</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251117</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251118</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251118</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251117</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251117</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251117</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251117</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251117</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251113</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251109</v>
+        <v>20251119</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Nov 19 23:24:27 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251117</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251118</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251117</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251117</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251117</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251117</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251117</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251118</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251118</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251117</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251117</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251117</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251117</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251117</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251113</v>
+        <v>20251120</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251111</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Nov 20 23:24:28 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251117</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251118</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251117</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251117</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251117</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251117</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251117</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251118</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251118</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251112</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251112</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251112</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251112</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251112</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251112</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251112</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251112</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251112</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251112</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251117</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251117</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251117</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251117</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251117</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251112</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251120</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251111</v>
+        <v>20251121</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Nov 21 23:24:25 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251117</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251118</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251117</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251117</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251117</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251117</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251117</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251118</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251113</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251113</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251113</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251113</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251113</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251113</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251113</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251113</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251118</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251117</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251117</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251117</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251117</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251117</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251112</v>
+        <v>20251122</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251120</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Nov 22 23:24:27 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251117</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251118</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251117</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251117</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251117</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251117</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251117</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251118</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251113</v>
+        <v>20251123</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251118</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251117</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251117</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251117</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251117</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251117</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251120</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Nov 23 23:23:59 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251115</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251115</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251115</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251115</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251115</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251115</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251115</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251115</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251115</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251115</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251118</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251115</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251115</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251118</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251118</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251115</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251117</v>
+        <v>20251124</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251120</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Nov 24 23:24:41 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251124</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251118</v>
+        <v>20251125</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251124</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251124</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251124</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251124</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251124</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251118</v>
+        <v>20251125</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251118</v>
+        <v>20251125</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251124</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251124</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251124</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251124</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251115</v>
+        <v>20251125</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251124</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251120</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Nov 25 23:24:59 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251124</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251125</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251124</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251124</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251124</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251124</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251124</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251125</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251117</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251117</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251117</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251125</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251117</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251117</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251117</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251124</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251124</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251124</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251124</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251124</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251120</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Nov 26 23:24:29 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251124</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251118</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251118</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251118</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251118</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251125</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251118</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251118</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251118</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251118</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251118</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251118</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251118</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251118</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251118</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251118</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251118</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251124</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251124</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251118</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251124</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251124</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251118</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251124</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251125</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251117</v>
+        <v>20251127</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251117</v>
+        <v>20251127</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251117</v>
+        <v>20251127</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251125</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251117</v>
+        <v>20251127</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251117</v>
+        <v>20251127</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251117</v>
+        <v>20251127</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251118</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251118</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251118</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251118</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251118</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251124</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251124</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251124</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251124</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251124</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251120</v>
+        <v>20251127</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Nov 27 23:24:14 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251124</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251119</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251125</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251124</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251124</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251124</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251124</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251124</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251125</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251125</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251118</v>
+        <v>20251128</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251119</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251119</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251119</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251119</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251119</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251119</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251119</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251124</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251124</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251124</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251124</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251124</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251127</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251119</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251119</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251119</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251119</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Nov 28 23:24:02 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251124</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251125</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251124</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251124</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251124</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251124</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251124</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251125</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251125</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251124</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251124</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251124</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251124</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251124</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251127</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251119</v>
+        <v>20251129</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Nov 29 23:24:26 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251117</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251117</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251117</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251117</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251117</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251124</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251117</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251117</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251117</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251117</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251125</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251124</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251124</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251124</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251124</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251124</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251125</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251125</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251124</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251124</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251124</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251124</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251124</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251127</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251121</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Nov 30 23:24:36 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251117</v>
+        <v>20251201</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251125</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251125</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251125</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251122</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251122</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251122</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251122</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251122</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251122</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251122</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251122</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251122</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251122</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251124</v>
+        <v>20251201</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251122</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251127</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251121</v>
+        <v>20251201</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Dec  1 23:25:31 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251201</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251125</v>
+        <v>20251202</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251201</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251201</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251201</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251201</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251201</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251125</v>
+        <v>20251202</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251123</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251123</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251123</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251123</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251123</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251123</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251123</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251123</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251125</v>
+        <v>20251202</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251201</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251201</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251201</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251201</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251201</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251122</v>
+        <v>20251202</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251127</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Dec  2 23:24:49 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251201</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251202</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251201</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251201</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251201</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251201</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251201</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251202</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251123</v>
+        <v>20251203</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251202</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251201</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251201</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251201</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251201</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251201</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251127</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Dec  3 23:23:48 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251125</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251125</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251125</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251201</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251125</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251125</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251125</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251125</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251125</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251125</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251125</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251202</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251201</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251201</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251125</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251201</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251125</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251201</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251201</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251202</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251202</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251201</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251201</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251201</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251201</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251125</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251201</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251127</v>
+        <v>20251204</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Dec  4 23:26:04 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251201</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251202</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251201</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251201</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251201</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251201</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251201</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251202</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251202</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251201</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251201</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251201</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251201</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251125</v>
+        <v>20251205</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251201</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251204</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Dec  5 23:25:30 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251201</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251202</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251201</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251201</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251201</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251201</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251201</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251202</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251127</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251127</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251127</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251202</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251127</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251127</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251127</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251201</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251201</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251201</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251201</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251201</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251204</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Dec  6 23:24:26 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251201</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251128</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251128</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251128</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251128</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251202</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251128</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251128</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251128</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251128</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251128</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251128</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251128</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251128</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251128</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251128</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251128</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251201</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251201</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251128</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251201</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251201</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251128</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251201</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251202</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251127</v>
+        <v>20251207</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251127</v>
+        <v>20251207</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251127</v>
+        <v>20251207</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251202</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251127</v>
+        <v>20251207</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251127</v>
+        <v>20251207</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251127</v>
+        <v>20251207</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251128</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251128</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251128</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251128</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251128</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251201</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251201</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251201</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251201</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251201</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251204</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Dec  7 23:23:51 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251129</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251202</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251202</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251202</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251128</v>
+        <v>20251208</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251129</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251129</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251129</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251129</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251129</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251129</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251129</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251201</v>
+        <v>20251208</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251204</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251129</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251129</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251129</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251129</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Dec  8 23:26:07 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251208</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251202</v>
+        <v>20251209</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251208</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251208</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251208</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251208</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251208</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251202</v>
+        <v>20251209</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251202</v>
+        <v>20251209</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251208</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251208</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251208</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251208</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251208</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251204</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251129</v>
+        <v>20251209</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Dec  9 23:26:47 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251208</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251209</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251208</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251208</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251208</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251208</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251208</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251209</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251209</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251208</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251208</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251208</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251208</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251208</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251204</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251201</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Dec 10 23:24:59 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251208</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251209</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251208</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251208</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251208</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251208</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251208</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251209</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251209</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251202</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251202</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251202</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251202</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251202</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251202</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251202</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251202</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251202</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251202</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251208</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251208</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251208</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251208</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251208</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251202</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251204</v>
+        <v>20251211</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251201</v>
+        <v>20251211</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Dec 11 23:26:44 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251208</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251209</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251208</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251208</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251208</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251208</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251208</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251209</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251203</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251203</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251203</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251203</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251203</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251203</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251203</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251203</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251209</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251208</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251208</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251208</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251208</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251208</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251202</v>
+        <v>20251212</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251211</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Dec 12 23:26:20 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251208</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251209</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251208</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251208</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251208</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251208</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251208</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251209</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251203</v>
+        <v>20251213</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251209</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251208</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251208</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251208</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251208</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251208</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251211</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Dec 13 23:24:56 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251201</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251201</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251201</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251205</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251201</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251205</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251201</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251205</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251208</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251201</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251205</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251201</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251201</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251201</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251205</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251205</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251205</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251205</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251205</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251205</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251209</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251208</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251208</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251205</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251208</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251205</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251208</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251208</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251209</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251209</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251208</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251208</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251208</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251208</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251205</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251208</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251211</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Dec 14 23:24:52 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251201</v>
+        <v>20251215</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251209</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251209</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251209</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251205</v>
+        <v>20251215</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251208</v>
+        <v>20251215</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251211</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Dec 15 23:27:04 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251215</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251209</v>
+        <v>20251216</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251215</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251215</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251215</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251215</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251215</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251209</v>
+        <v>20251216</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251207</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251207</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251207</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251209</v>
+        <v>20251216</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251207</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251207</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251207</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251215</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251215</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251215</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251215</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251215</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251211</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Dec 16 23:26:42 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251215</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251208</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251208</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251208</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251208</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251216</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251208</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251208</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251208</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251208</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251208</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251208</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251208</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251208</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251208</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251208</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251208</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251215</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251215</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251208</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251215</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251215</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251208</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251215</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251216</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251207</v>
+        <v>20251217</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251207</v>
+        <v>20251217</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251207</v>
+        <v>20251217</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251216</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251207</v>
+        <v>20251217</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251207</v>
+        <v>20251217</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251207</v>
+        <v>20251217</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251208</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251208</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251208</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251208</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251208</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251215</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251215</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251215</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251215</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251215</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251211</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Dec 17 23:26:47 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251215</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251209</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251216</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251215</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251215</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251215</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251215</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251215</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251216</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251216</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251208</v>
+        <v>20251218</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251209</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251209</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251209</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251209</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251209</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251209</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251209</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251215</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251215</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251215</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251215</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251215</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251211</v>
+        <v>20251218</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251209</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251209</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251209</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251209</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Dec 18 23:26:36 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251215</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251216</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251215</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251215</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251215</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251215</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251215</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251216</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251216</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251215</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251215</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251215</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251215</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251215</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251218</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251209</v>
+        <v>20251219</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Dec 19 23:25:59 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251215</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251216</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251215</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251215</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251215</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251215</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251215</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251216</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251216</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251215</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251215</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251215</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251215</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251215</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251218</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251211</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Dec 20 23:24:25 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251215</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251216</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251215</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251215</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251215</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251215</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251215</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251216</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251216</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251212</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251212</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251212</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251212</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251212</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251212</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251212</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251212</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251212</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251212</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251215</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251215</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251215</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251215</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251215</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251212</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251218</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251211</v>
+        <v>20251221</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Dec 21 23:25:14 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251216</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251216</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251213</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251213</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251213</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251213</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251213</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251213</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251213</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251213</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251216</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251215</v>
+        <v>20251222</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251212</v>
+        <v>20251222</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251218</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Dec 22 23:26:14 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251222</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251216</v>
+        <v>20251223</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251222</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251222</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251222</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251222</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251222</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251216</v>
+        <v>20251223</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251213</v>
+        <v>20251223</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251216</v>
+        <v>20251223</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251222</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251222</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251222</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251222</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251222</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251218</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Dec 23 23:25:51 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251215</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251215</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251215</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251222</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251215</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251215</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251215</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251215</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251215</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251215</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251215</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251223</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251222</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251222</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251215</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251222</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251215</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251222</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251222</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251223</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251223</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251222</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251222</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251222</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251222</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251215</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251222</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251218</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Dec 24 23:26:04 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251222</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251223</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251222</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251222</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251222</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251222</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251222</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251223</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251223</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251222</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251222</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251222</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251222</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251215</v>
+        <v>20251225</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251222</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251218</v>
+        <v>20251225</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Dec 25 23:26:28 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251222</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251223</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251222</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251222</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251222</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251222</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251222</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251223</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251217</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251217</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251217</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251223</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251217</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251217</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251217</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251222</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251222</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251222</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251222</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251222</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20251225</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Dec 26 23:26:20 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251222</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251218</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251218</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251218</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251218</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251223</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251218</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251218</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251218</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251218</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251218</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251218</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251218</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251218</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251218</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251218</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251218</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251222</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251222</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251218</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251222</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251222</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251218</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251222</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251223</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251217</v>
+        <v>20251227</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251217</v>
+        <v>20251227</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251217</v>
+        <v>20251227</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251223</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251217</v>
+        <v>20251227</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251217</v>
+        <v>20251227</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251217</v>
+        <v>20251227</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251218</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251218</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251218</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251218</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251218</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251222</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251222</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251222</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251222</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251222</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20251225</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Dec 27 23:25:23 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251215</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251215</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251215</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251215</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251215</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251222</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251215</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251215</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251215</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251215</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251219</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251223</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251222</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251222</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251222</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251222</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251222</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251223</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251223</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251218</v>
+        <v>20251228</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251219</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251219</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251219</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251219</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251219</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251219</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251219</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251222</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251222</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251222</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251222</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251222</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20251225</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251219</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251219</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251219</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251219</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Dec 28 23:26:15 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251215</v>
+        <v>20251229</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251223</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251223</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251223</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251222</v>
+        <v>20251229</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20251225</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251219</v>
+        <v>20251229</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Dec 29 23:26:22 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20251229</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251223</v>
+        <v>20251230</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20251229</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20251229</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20251229</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20251229</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20251229</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251223</v>
+        <v>20251230</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251223</v>
+        <v>20251230</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20251229</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20251229</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20251229</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20251229</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20251229</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20251225</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251221</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Dec 30 23:25:43 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20251229</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20251230</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20251229</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20251229</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20251229</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20251229</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20251229</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20251230</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20251230</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20251222</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20251222</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20251222</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20251222</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20251222</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20251222</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20251222</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20251222</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20251222</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20251222</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20251229</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20251229</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20251229</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20251229</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20251229</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20251222</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20251225</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251221</v>
+        <v>20251231</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Dec 31 23:26:36 UTC 2025
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20251229</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20251230</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20251229</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20251229</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20251229</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20251229</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20251229</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20251230</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20251223</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20251223</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20251223</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20251223</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20251223</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20251223</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20251223</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20251223</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20251230</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20251229</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20251229</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20251229</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20251229</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20251229</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20251222</v>
+        <v>20260101</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20251225</v>
+        <v>20260101</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Jan  1 23:26:58 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20251229</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20251230</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20251229</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20251229</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20251229</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20251229</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20251229</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20251230</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20251223</v>
+        <v>20260102</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20251230</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20251229</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20251229</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20251229</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20251229</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20251229</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20260101</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Jan  2 23:26:35 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20251225</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20251225</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20251225</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20251229</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20251225</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20251225</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20251225</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20251225</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20251225</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20251225</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20251225</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20251230</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20251229</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20251229</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20251225</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20251229</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20251225</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20251229</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20251229</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20251230</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20251230</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20251229</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20251229</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20251229</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20251229</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20251225</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20251229</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20260101</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Jan  3 23:26:16 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20251229</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20251230</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20251229</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20251229</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20251229</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20251229</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20251229</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20251230</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20251230</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20251229</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20251229</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20251229</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20251229</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20251225</v>
+        <v>20260104</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20251229</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20260101</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Jan  4 23:26:31 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20251230</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20251230</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20251227</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20251227</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20251227</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20251230</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20251227</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20251227</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20251227</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20251229</v>
+        <v>20260105</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20260101</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Jan  5 23:27:40 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20260105</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20251228</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20251228</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20251228</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20251228</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20251230</v>
+        <v>20260106</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20251228</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20251228</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20251228</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20251228</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20251228</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20251228</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20251228</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20251228</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20251228</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20251228</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20251228</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20260105</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20260105</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20251228</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20260105</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20260105</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20251228</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20260105</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20251230</v>
+        <v>20260106</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20251227</v>
+        <v>20260106</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20251227</v>
+        <v>20260106</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20251227</v>
+        <v>20260106</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20251230</v>
+        <v>20260106</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20251227</v>
+        <v>20260106</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20251227</v>
+        <v>20260106</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20251227</v>
+        <v>20260106</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20251228</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20251228</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20251228</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20251228</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20251228</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20260105</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20260105</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20260105</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20260105</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20260105</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20260101</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Jan  6 23:27:56 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20260105</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20251229</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20260106</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20260105</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20260105</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20260105</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20260105</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20260105</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20260106</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20260106</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20251228</v>
+        <v>20260107</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20251229</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20251229</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20251229</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20251229</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20251229</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20251229</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20251229</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20260105</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20260105</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20260105</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20260105</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20260105</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20260101</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20251229</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20251229</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20251229</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20251229</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Jan  7 23:28:00 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20260105</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20260106</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20260105</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20260105</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20260105</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20260105</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20260105</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20260106</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20260106</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20260105</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20260105</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20260105</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20260105</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20260105</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20260101</v>
+        <v>20260108</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20251229</v>
+        <v>20260108</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Jan  8 23:24:55 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20260105</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20260106</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20260105</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20260105</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20260105</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20260105</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20260105</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20260106</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20260106</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20260105</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20260105</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20260105</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20260105</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20260105</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20260108</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20251231</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Jan  9 23:27:37 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20260105</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20260106</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20260105</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20260105</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20260105</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20260105</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20260105</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20260106</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20260106</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20260101</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20260101</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20260101</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20260101</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20260101</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20260101</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20260101</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20260101</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20260101</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20260101</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20260105</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20260105</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20260105</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20260105</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20260105</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20260101</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20260108</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20251231</v>
+        <v>20260110</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Jan 10 23:26:04 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20251229</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>20251229</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>20251229</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>20251229</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>20251229</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20260105</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>20251229</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>20251229</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>20251229</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>20251229</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20260106</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20260105</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20260105</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20260105</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20260105</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20260105</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20260106</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20260102</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20260102</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20260102</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20260102</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20260102</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20260102</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20260102</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20260102</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20260106</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20260105</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20260105</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20260105</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20260105</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20260105</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20260101</v>
+        <v>20260111</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20260108</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Jan 11 23:26:13 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,10 +638,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,10 +793,10 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -890,10 +890,10 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -925,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20251229</v>
+        <v>20260112</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20260106</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20260106</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20260102</v>
+        <v>20260112</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20260106</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20260105</v>
+        <v>20260112</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20260108</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Jan 12 23:23:19 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20260104</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20260104</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20260104</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20260112</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20260104</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20260104</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20260104</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20260104</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20260104</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20260104</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20260104</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20260106</v>
+        <v>20260113</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20260112</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20260112</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20260104</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20260112</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20260104</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20260112</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20260112</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20260106</v>
+        <v>20260113</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20260106</v>
+        <v>20260113</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20260112</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20260112</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20260112</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20260112</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20260104</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20260112</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20260108</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Jan 13 23:25:59 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20260112</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20260113</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20260112</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20260112</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20260112</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20260112</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20260112</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20260113</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20260113</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20260112</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20260112</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20260112</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20260112</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20260104</v>
+        <v>20260114</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20260112</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20260108</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Jan 14 23:24:27 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20260112</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20260113</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20260112</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20260112</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20260112</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20260112</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20260112</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20260113</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
         <v>20260106</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="n">
         <v>20260106</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F60" t="n">
         <v>20260106</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20260113</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
         <v>20260106</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="n">
         <v>20260106</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" t="n">
         <v>20260106</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20260112</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20260112</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20260112</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20260112</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20260112</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20260108</v>
+        <v>20260115</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Jan 15 23:28:35 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20260112</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>20260107</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>20260107</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>20260107</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>20260107</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20260113</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>20260107</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
         <v>20260107</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>20260107</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>20260107</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>20260107</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
         <v>20260107</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
         <v>20260107</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>20260107</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
         <v>20260107</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>20260107</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
         <v>20260107</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20260112</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20260112</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>20260107</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20260112</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20260112</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
         <v>20260107</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20260112</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20260113</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,10 +2278,10 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>20260106</v>
+        <v>20260116</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
@@ -2309,10 +2309,10 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>20260106</v>
+        <v>20260116</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2340,10 +2340,10 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>20260106</v>
+        <v>20260116</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20260113</v>
@@ -2402,10 +2402,10 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>20260106</v>
+        <v>20260116</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2433,10 +2433,10 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>20260106</v>
+        <v>20260116</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2464,10 +2464,10 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>20260106</v>
+        <v>20260116</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
         <v>20260107</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>20260107</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="n">
         <v>20260107</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>20260107</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="n">
         <v>20260107</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20260112</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20260112</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20260112</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20260112</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20260112</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20260115</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Jan 16 23:27:22 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20260112</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>20260108</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1084,10 +1084,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20260113</v>
@@ -1336,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1367,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1429,10 +1429,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1491,10 +1491,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1522,10 +1522,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1619,10 +1619,10 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1650,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1681,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20260112</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20260112</v>
@@ -1778,10 +1778,10 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20260112</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20260112</v>
@@ -1937,10 +1937,10 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20260112</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20260113</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20260113</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,10 +2495,10 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2526,10 +2526,10 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
@@ -2557,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
@@ -2588,10 +2588,10 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2619,10 +2619,10 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>20260107</v>
+        <v>20260117</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
         <v>20260108</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="n">
         <v>20260108</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
         <v>20260108</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="n">
         <v>20260108</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" t="n">
         <v>20260108</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="n">
         <v>20260108</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>20260108</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20260112</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20260112</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20260112</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20260112</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20260112</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20260115</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>20260108</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="n">
         <v>20260108</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F98" t="n">
         <v>20260108</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="n">
         <v>20260108</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Jan 17 23:26:05 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>20260112</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,10 +960,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>20260113</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>20260112</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>20260112</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>20260112</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>20260112</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
         <v>20260112</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="n">
         <v>20260113</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>20260113</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,10 +2650,10 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2681,10 +2681,10 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2712,10 +2712,10 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2743,10 +2743,10 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2774,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2805,10 +2805,10 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F75" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2836,10 +2836,10 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="n">
         <v>20260112</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>20260112</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="n">
         <v>20260112</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" t="n">
         <v>20260112</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" t="n">
         <v>20260112</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
         <v>20260115</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,10 +3456,10 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F96" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr">
@@ -3487,10 +3487,10 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F97" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3518,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3549,10 +3549,10 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>20260108</v>
+        <v>20260118</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sun Jan 18 23:26:50 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,10 +762,10 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>20260113</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,10 +1716,10 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,10 +1902,10 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,10 +1968,10 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F48" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
         <v>20260113</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>20260113</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3208,10 +3208,10 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
@@ -3239,10 +3239,10 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F89" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
@@ -3270,10 +3270,10 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F90" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F92" t="n">
-        <v>20260112</v>
+        <v>20260119</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
         <v>20260115</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="n">
         <v>20260110</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Mon Jan 19 23:28:14 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>20260119</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,10 +1301,10 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>20260113</v>
+        <v>20260120</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
         <v>20260119</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" t="n">
         <v>20260119</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
         <v>20260119</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>20260119</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
         <v>20260119</v>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
-        <v>20260113</v>
+        <v>20260120</v>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F61" t="n">
-        <v>20260113</v>
+        <v>20260120</v>
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>20260111</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
         <v>20260111</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
         <v>20260111</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F80" t="n">
         <v>20260111</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="n">
         <v>20260111</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" t="n">
         <v>20260111</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>20260111</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>20260111</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
         <v>20260111</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="n">
         <v>20260111</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" t="n">
         <v>20260119</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" t="n">
         <v>20260119</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" t="n">
         <v>20260119</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
         <v>20260119</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
         <v>20260119</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="n">
         <v>20260111</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F94" t="n">
         <v>20260115</v>
@@ -3425,10 +3425,10 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F95" t="n">
-        <v>20260110</v>
+        <v>20260120</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Tue Jan 20 23:30:10 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>20260119</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
         <v>20260120</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F40" t="n">
         <v>20260119</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
         <v>20260119</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F44" t="n">
         <v>20260119</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
         <v>20260119</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48" t="n">
         <v>20260119</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>20260120</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
         <v>20260112</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
         <v>20260112</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
         <v>20260112</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
         <v>20260112</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>20260112</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
         <v>20260112</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
         <v>20260112</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
         <v>20260112</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" t="n">
         <v>20260120</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,10 +2867,10 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F77" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2929,10 +2929,10 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2960,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F80" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2991,10 +2991,10 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -3022,10 +3022,10 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
@@ -3053,10 +3053,10 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F83" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
@@ -3084,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
@@ -3146,10 +3146,10 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F86" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
         <v>20260119</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" t="n">
         <v>20260119</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
         <v>20260119</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F90" t="n">
         <v>20260119</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" t="n">
         <v>20260119</v>
@@ -3363,10 +3363,10 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F93" t="n">
-        <v>20260111</v>
+        <v>20260121</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F94" t="n">
         <v>20260115</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>20260120</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Wed Jan 21 23:32:41 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>20260119</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
         <v>20260120</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
         <v>20260119</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" t="n">
         <v>20260119</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>20260119</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>20260119</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
         <v>20260119</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
         <v>20260120</v>
@@ -2030,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2092,10 +2092,10 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2185,10 +2185,10 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F55" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2216,10 +2216,10 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
@@ -2247,10 +2247,10 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" t="n">
-        <v>20260112</v>
+        <v>20260122</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>20260120</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" t="n">
         <v>20260121</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78" t="n">
         <v>20260121</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
         <v>20260121</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" t="n">
         <v>20260121</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81" t="n">
         <v>20260121</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82" t="n">
         <v>20260121</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
         <v>20260121</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" t="n">
         <v>20260121</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" t="n">
         <v>20260121</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" t="n">
         <v>20260121</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F87" t="n">
         <v>20260119</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="n">
         <v>20260119</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F89" t="n">
         <v>20260119</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
         <v>20260119</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>20260119</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F93" t="n">
         <v>20260121</v>
@@ -3394,10 +3394,10 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F94" t="n">
-        <v>20260115</v>
+        <v>20260122</v>
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F95" t="n">
         <v>20260120</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Thu Jan 22 23:28:59 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>20260114</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>20260114</v>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>20260114</v>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>20260119</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>20260114</v>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>20260114</v>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>20260114</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>20260114</v>
@@ -1208,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>20260114</v>
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>20260114</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>20260114</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>20260120</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40" t="n">
         <v>20260119</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="n">
         <v>20260119</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>20260114</v>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
         <v>20260119</v>
@@ -1871,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>20260114</v>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>20260119</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48" t="n">
         <v>20260119</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F49" t="n">
         <v>20260120</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="n">
         <v>20260122</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="n">
         <v>20260122</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" t="n">
         <v>20260122</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
         <v>20260122</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
         <v>20260122</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" t="n">
         <v>20260122</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>20260122</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" t="n">
         <v>20260122</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
         <v>20260120</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
         <v>20260121</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
         <v>20260121</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="n">
         <v>20260121</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
         <v>20260121</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="n">
         <v>20260121</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
         <v>20260121</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
         <v>20260121</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
         <v>20260121</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
         <v>20260121</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="n">
         <v>20260121</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
         <v>20260119</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
         <v>20260119</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
         <v>20260119</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
         <v>20260119</v>
@@ -3301,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="n">
         <v>20260114</v>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="n">
         <v>20260119</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
         <v>20260121</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" t="n">
         <v>20260122</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
         <v>20260120</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Fri Jan 23 23:28:49 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>20260112</v>
@@ -568,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>20260112</v>
@@ -603,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>20260112</v>
@@ -669,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>20260112</v>
@@ -731,10 +731,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>20260119</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
         <v>20260112</v>
@@ -824,10 +824,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>20260112</v>
@@ -890,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>20260112</v>
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>20260112</v>
@@ -960,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>20260118</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>20260117</v>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
         <v>20260117</v>
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>20260117</v>
@@ -1115,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>20260117</v>
@@ -1146,10 +1146,10 @@
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1177,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1208,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1239,10 +1239,10 @@
         <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1270,10 +1270,10 @@
         <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>20260120</v>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
         <v>20260117</v>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>20260117</v>
@@ -1398,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
         <v>20260117</v>
@@ -1429,7 +1429,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31" t="n">
         <v>20260117</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>20260117</v>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
         <v>20260117</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" t="n">
         <v>20260117</v>
@@ -1557,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
         <v>20260117</v>
@@ -1619,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37" t="n">
         <v>20260117</v>
@@ -1650,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="n">
         <v>20260117</v>
@@ -1681,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="E39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>20260117</v>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
         <v>20260119</v>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
         <v>20260119</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>20260117</v>
@@ -1809,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
         <v>20260119</v>
@@ -1871,10 +1871,10 @@
         <v>10</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="n">
         <v>20260119</v>
@@ -1937,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
         <v>20260117</v>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
         <v>20260119</v>
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="E49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
         <v>20260120</v>
@@ -2030,7 +2030,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
         <v>20260122</v>
@@ -2061,7 +2061,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="n">
         <v>20260122</v>
@@ -2092,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
         <v>20260122</v>
@@ -2123,7 +2123,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="n">
         <v>20260122</v>
@@ -2154,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="n">
         <v>20260122</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
         <v>20260122</v>
@@ -2216,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="n">
         <v>20260122</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="E57" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="n">
         <v>20260122</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>20260116</v>
@@ -2309,7 +2309,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
         <v>20260116</v>
@@ -2340,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="n">
         <v>20260116</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" t="n">
         <v>20260120</v>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>20260116</v>
@@ -2433,7 +2433,7 @@
         <v>10</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
         <v>20260116</v>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
         <v>20260116</v>
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>20260117</v>
@@ -2526,7 +2526,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
         <v>20260117</v>
@@ -2557,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F67" t="n">
         <v>20260117</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
         <v>20260117</v>
@@ -2619,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="E69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
         <v>20260117</v>
@@ -2650,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>20260118</v>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F71" t="n">
         <v>20260118</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
         <v>20260118</v>
@@ -2743,7 +2743,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
         <v>20260118</v>
@@ -2774,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
         <v>20260118</v>
@@ -2805,7 +2805,7 @@
         <v>10</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>20260118</v>
@@ -2836,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="E76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="n">
         <v>20260118</v>
@@ -2867,7 +2867,7 @@
         <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F77" t="n">
         <v>20260121</v>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
         <v>20260121</v>
@@ -2929,7 +2929,7 @@
         <v>10</v>
       </c>
       <c r="E79" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F79" t="n">
         <v>20260121</v>
@@ -2960,7 +2960,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
         <v>20260121</v>
@@ -2991,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="E81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F81" t="n">
         <v>20260121</v>
@@ -3022,7 +3022,7 @@
         <v>10</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
         <v>20260121</v>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
         <v>20260121</v>
@@ -3084,7 +3084,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84" t="n">
         <v>20260121</v>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
         <v>20260121</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F86" t="n">
         <v>20260121</v>
@@ -3177,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" t="n">
         <v>20260119</v>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88" t="n">
         <v>20260119</v>
@@ -3239,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F89" t="n">
         <v>20260119</v>
@@ -3270,7 +3270,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
         <v>20260119</v>
@@ -3301,10 +3301,10 @@
         <v>10</v>
       </c>
       <c r="E91" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>20260114</v>
+        <v>20260124</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
         <v>20260119</v>
@@ -3363,7 +3363,7 @@
         <v>10</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F93" t="n">
         <v>20260121</v>
@@ -3394,7 +3394,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" t="n">
         <v>20260122</v>
@@ -3425,7 +3425,7 @@
         <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="n">
         <v>20260120</v>
@@ -3456,7 +3456,7 @@
         <v>10</v>
       </c>
       <c r="E96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="n">
         <v>20260118</v>
@@ -3487,7 +3487,7 @@
         <v>10</v>
       </c>
       <c r="E97" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F97" t="n">
         <v>20260118</v>
@@ -3518,7 +3518,7 @@
         <v>10</v>
       </c>
       <c r="E98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="n">
         <v>20260118</v>
@@ -3549,7 +3549,7 @@
         <v>10</v>
       </c>
       <c r="E99" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F99" t="n">
         <v>20260118</v>

</xml_diff>

<commit_message>
自动更新Excel文件 - Sat Jan 24 23:26:56 UTC 2026
</commit_message>
<xml_diff>
--- a/yxc_backup.xlsx
+++ b/yxc_backup.xlsx
@@ -498,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>20260112</v>
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+